<commit_message>
Cambios en la plantilla
Se agregan plantillas para los requerimientos.
</commit_message>
<xml_diff>
--- a/documentos/Plantillas análisis.xlsx
+++ b/documentos/Plantillas análisis.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SyncHostel\synchostel\documentos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Dvlpmnt\synchostel\documentos\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1350" windowWidth="20490" windowHeight="7890" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="1350" windowWidth="20490" windowHeight="7890" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Actor" sheetId="1" r:id="rId1"/>
     <sheet name="Caso de uso narrativo" sheetId="2" r:id="rId2"/>
+    <sheet name="Requerimientos" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -695,8 +696,211 @@
 </comments>
 </file>
 
+<file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Ivan</author>
+  </authors>
+  <commentList>
+    <comment ref="D5" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Ivan:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Al lado del ID se le asignará un número al requerimiento. Por ejemplo, ID1. En el recuadro de al lado se pondrá el nombre del requerimiento.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D6" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Ivan:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Se indica la fecha en la que escribimos el requerimiento, si se modifica posteriormente, se le cambia la fecha</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D7" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Ivan:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Requisitos de los que depende este requisito</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D8" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Ivan:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Descripción del requerimiento.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D9" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Ivan:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Importancia del CLIENTE para el cumplimiento de este requerimiento.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D10" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Ivan:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Prioridad que tiene para el equipo de desarrollo.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D11" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Ivan:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Estado de vida según el largo del proyecto.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D12" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Ivan:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Comentarios……………..???
+</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="33">
   <si>
     <t>Actor</t>
   </si>
@@ -780,6 +984,21 @@
   </si>
   <si>
     <t>Estabilidad</t>
+  </si>
+  <si>
+    <t>Requerimientos</t>
+  </si>
+  <si>
+    <t>Versión</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>Dependencias</t>
+  </si>
+  <si>
+    <t>Prioridad</t>
   </si>
 </sst>
 </file>
@@ -847,7 +1066,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="29">
+  <borders count="33">
     <border>
       <left/>
       <right/>
@@ -1231,31 +1450,78 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="67">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1265,16 +1531,30 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1287,51 +1567,53 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1615,7 +1897,7 @@
   <dimension ref="B1:G15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1634,130 +1916,135 @@
       <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="4" t="s">
+      <c r="C2" s="33"/>
+      <c r="D2" s="33"/>
+      <c r="E2" s="33"/>
+      <c r="F2" s="33"/>
+      <c r="G2" s="3" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="3" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="6"/>
-      <c r="D3" s="7"/>
-      <c r="E3" s="7"/>
-      <c r="F3" s="7"/>
-      <c r="G3" s="8"/>
+      <c r="C3" s="25"/>
+      <c r="D3" s="26"/>
+      <c r="E3" s="26"/>
+      <c r="F3" s="26"/>
+      <c r="G3" s="32"/>
     </row>
     <row r="4" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="6"/>
-      <c r="D4" s="7"/>
-      <c r="E4" s="7"/>
-      <c r="F4" s="7"/>
-      <c r="G4" s="8"/>
+      <c r="C4" s="25"/>
+      <c r="D4" s="26"/>
+      <c r="E4" s="26"/>
+      <c r="F4" s="26"/>
+      <c r="G4" s="32"/>
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="6"/>
-      <c r="D5" s="7"/>
-      <c r="E5" s="7"/>
-      <c r="F5" s="7"/>
-      <c r="G5" s="8"/>
+      <c r="C5" s="25"/>
+      <c r="D5" s="26"/>
+      <c r="E5" s="26"/>
+      <c r="F5" s="26"/>
+      <c r="G5" s="32"/>
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="6"/>
-      <c r="D6" s="7"/>
-      <c r="E6" s="7"/>
-      <c r="F6" s="7"/>
-      <c r="G6" s="8"/>
+      <c r="C6" s="25"/>
+      <c r="D6" s="26"/>
+      <c r="E6" s="26"/>
+      <c r="F6" s="26"/>
+      <c r="G6" s="32"/>
     </row>
     <row r="7" spans="2:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="9" t="s">
+      <c r="B7" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="10"/>
-      <c r="D7" s="10" t="s">
+      <c r="C7" s="6"/>
+      <c r="D7" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="E7" s="10"/>
-      <c r="F7" s="10" t="s">
+      <c r="E7" s="6"/>
+      <c r="F7" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="G7" s="11"/>
+      <c r="G7" s="7"/>
     </row>
     <row r="8" spans="2:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="9" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B9" s="12" t="s">
+      <c r="B9" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="C9" s="13"/>
-      <c r="D9" s="13"/>
-      <c r="E9" s="13"/>
-      <c r="F9" s="13"/>
-      <c r="G9" s="14"/>
+      <c r="C9" s="18"/>
+      <c r="D9" s="18"/>
+      <c r="E9" s="18"/>
+      <c r="F9" s="18"/>
+      <c r="G9" s="19"/>
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B10" s="5" t="s">
+      <c r="B10" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C10" s="15" t="s">
+      <c r="C10" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="D10" s="15"/>
-      <c r="E10" s="15"/>
-      <c r="F10" s="15" t="s">
+      <c r="D10" s="23"/>
+      <c r="E10" s="23"/>
+      <c r="F10" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="G10" s="16"/>
+      <c r="G10" s="24"/>
     </row>
     <row r="11" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B11" s="5"/>
-      <c r="C11" s="6"/>
-      <c r="D11" s="7"/>
-      <c r="E11" s="17"/>
-      <c r="F11" s="6"/>
-      <c r="G11" s="8"/>
+      <c r="B11" s="4"/>
+      <c r="C11" s="25"/>
+      <c r="D11" s="26"/>
+      <c r="E11" s="27"/>
+      <c r="F11" s="25"/>
+      <c r="G11" s="32"/>
     </row>
     <row r="12" spans="2:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="18"/>
-      <c r="C12" s="19"/>
-      <c r="D12" s="20"/>
-      <c r="E12" s="21"/>
-      <c r="F12" s="19"/>
-      <c r="G12" s="22"/>
+      <c r="B12" s="8"/>
+      <c r="C12" s="28"/>
+      <c r="D12" s="29"/>
+      <c r="E12" s="30"/>
+      <c r="F12" s="28"/>
+      <c r="G12" s="31"/>
     </row>
     <row r="13" spans="2:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="14" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B14" s="12" t="s">
+      <c r="B14" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="C14" s="13"/>
-      <c r="D14" s="13"/>
-      <c r="E14" s="13"/>
-      <c r="F14" s="13"/>
-      <c r="G14" s="14"/>
+      <c r="C14" s="18"/>
+      <c r="D14" s="18"/>
+      <c r="E14" s="18"/>
+      <c r="F14" s="18"/>
+      <c r="G14" s="19"/>
     </row>
     <row r="15" spans="2:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="23"/>
-      <c r="C15" s="24"/>
-      <c r="D15" s="24"/>
-      <c r="E15" s="24"/>
-      <c r="F15" s="24"/>
-      <c r="G15" s="25"/>
+      <c r="B15" s="20"/>
+      <c r="C15" s="21"/>
+      <c r="D15" s="21"/>
+      <c r="E15" s="21"/>
+      <c r="F15" s="21"/>
+      <c r="G15" s="22"/>
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="C2:F2"/>
+    <mergeCell ref="C3:G3"/>
+    <mergeCell ref="C4:G4"/>
+    <mergeCell ref="C5:G5"/>
+    <mergeCell ref="C6:G6"/>
     <mergeCell ref="B14:G14"/>
     <mergeCell ref="B15:G15"/>
     <mergeCell ref="C10:E10"/>
@@ -1767,11 +2054,6 @@
     <mergeCell ref="C12:E12"/>
     <mergeCell ref="F12:G12"/>
     <mergeCell ref="F11:G11"/>
-    <mergeCell ref="C2:F2"/>
-    <mergeCell ref="C3:G3"/>
-    <mergeCell ref="C4:G4"/>
-    <mergeCell ref="C5:G5"/>
-    <mergeCell ref="C6:G6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -1783,8 +2065,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:I30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="L26" sqref="L26"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E45" sqref="E45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1799,319 +2081,298 @@
     <col min="9" max="16384" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:9" s="1" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="26" t="s">
+    <row r="1" spans="2:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B2" s="50" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="27"/>
-      <c r="D2" s="28"/>
-      <c r="E2" s="29"/>
-      <c r="F2" s="27"/>
-      <c r="G2" s="27"/>
-      <c r="H2" s="28"/>
-      <c r="I2" s="4" t="s">
+      <c r="C2" s="37"/>
+      <c r="D2" s="38"/>
+      <c r="E2" s="36"/>
+      <c r="F2" s="37"/>
+      <c r="G2" s="37"/>
+      <c r="H2" s="38"/>
+      <c r="I2" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="2:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="30" t="s">
+    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B3" s="52" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="31"/>
-      <c r="D3" s="32"/>
-      <c r="E3" s="33"/>
-      <c r="F3" s="33"/>
-      <c r="G3" s="33"/>
-      <c r="H3" s="33"/>
-      <c r="I3" s="34"/>
-    </row>
-    <row r="4" spans="2:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="30" t="s">
+      <c r="C3" s="53"/>
+      <c r="D3" s="54"/>
+      <c r="E3" s="34"/>
+      <c r="F3" s="34"/>
+      <c r="G3" s="34"/>
+      <c r="H3" s="34"/>
+      <c r="I3" s="35"/>
+    </row>
+    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B4" s="52" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="31"/>
-      <c r="D4" s="32"/>
-      <c r="E4" s="33"/>
-      <c r="F4" s="33"/>
-      <c r="G4" s="33"/>
-      <c r="H4" s="33"/>
-      <c r="I4" s="34"/>
-    </row>
-    <row r="5" spans="2:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="30" t="s">
+      <c r="C4" s="53"/>
+      <c r="D4" s="54"/>
+      <c r="E4" s="34"/>
+      <c r="F4" s="34"/>
+      <c r="G4" s="34"/>
+      <c r="H4" s="34"/>
+      <c r="I4" s="35"/>
+    </row>
+    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B5" s="52" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="31"/>
-      <c r="D5" s="32"/>
-      <c r="E5" s="35"/>
-      <c r="F5" s="15"/>
-      <c r="G5" s="15"/>
-      <c r="H5" s="15"/>
-      <c r="I5" s="16"/>
-    </row>
-    <row r="6" spans="2:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="30" t="s">
+      <c r="C5" s="53"/>
+      <c r="D5" s="54"/>
+      <c r="E5" s="13"/>
+      <c r="F5" s="23"/>
+      <c r="G5" s="23"/>
+      <c r="H5" s="23"/>
+      <c r="I5" s="24"/>
+    </row>
+    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B6" s="52" t="s">
         <v>15</v>
       </c>
-      <c r="C6" s="31"/>
-      <c r="D6" s="32"/>
-      <c r="E6" s="33"/>
-      <c r="F6" s="33"/>
-      <c r="G6" s="33"/>
-      <c r="H6" s="33"/>
-      <c r="I6" s="34"/>
-    </row>
-    <row r="7" spans="2:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="30" t="s">
+      <c r="C6" s="53"/>
+      <c r="D6" s="54"/>
+      <c r="E6" s="34"/>
+      <c r="F6" s="34"/>
+      <c r="G6" s="34"/>
+      <c r="H6" s="34"/>
+      <c r="I6" s="35"/>
+    </row>
+    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B7" s="52" t="s">
         <v>16</v>
       </c>
-      <c r="C7" s="31"/>
-      <c r="D7" s="32"/>
-      <c r="E7" s="33"/>
-      <c r="F7" s="33"/>
-      <c r="G7" s="33"/>
-      <c r="H7" s="33"/>
-      <c r="I7" s="34"/>
-    </row>
-    <row r="8" spans="2:9" s="1" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="36" t="s">
+      <c r="C7" s="53"/>
+      <c r="D7" s="54"/>
+      <c r="E7" s="34"/>
+      <c r="F7" s="34"/>
+      <c r="G7" s="34"/>
+      <c r="H7" s="34"/>
+      <c r="I7" s="35"/>
+    </row>
+    <row r="8" spans="2:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="55" t="s">
         <v>4</v>
       </c>
-      <c r="C8" s="37"/>
-      <c r="D8" s="38"/>
-      <c r="E8" s="10"/>
-      <c r="F8" s="10" t="s">
+      <c r="C8" s="56"/>
+      <c r="D8" s="57"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="G8" s="10"/>
-      <c r="H8" s="10" t="s">
+      <c r="G8" s="6"/>
+      <c r="H8" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="I8" s="11"/>
-    </row>
-    <row r="9" spans="2:9" s="1" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="10" spans="2:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="39" t="s">
+      <c r="I8" s="7"/>
+    </row>
+    <row r="9" spans="2:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B10" s="43" t="s">
         <v>17</v>
       </c>
-      <c r="C10" s="40"/>
-      <c r="D10" s="40"/>
-      <c r="E10" s="40"/>
-      <c r="F10" s="40"/>
-      <c r="G10" s="40"/>
-      <c r="H10" s="40"/>
-      <c r="I10" s="41"/>
-    </row>
-    <row r="11" spans="2:9" s="1" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="42"/>
-      <c r="C11" s="43"/>
-      <c r="D11" s="43"/>
-      <c r="E11" s="43"/>
-      <c r="F11" s="43"/>
-      <c r="G11" s="43"/>
-      <c r="H11" s="43"/>
-      <c r="I11" s="44"/>
-    </row>
-    <row r="12" spans="2:9" s="1" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="13" spans="2:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="39" t="s">
+      <c r="C10" s="44"/>
+      <c r="D10" s="44"/>
+      <c r="E10" s="44"/>
+      <c r="F10" s="44"/>
+      <c r="G10" s="44"/>
+      <c r="H10" s="44"/>
+      <c r="I10" s="45"/>
+    </row>
+    <row r="11" spans="2:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="46"/>
+      <c r="C11" s="39"/>
+      <c r="D11" s="39"/>
+      <c r="E11" s="39"/>
+      <c r="F11" s="39"/>
+      <c r="G11" s="39"/>
+      <c r="H11" s="39"/>
+      <c r="I11" s="41"/>
+    </row>
+    <row r="12" spans="2:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B13" s="43" t="s">
         <v>18</v>
       </c>
-      <c r="C13" s="40"/>
-      <c r="D13" s="40"/>
-      <c r="E13" s="40"/>
-      <c r="F13" s="40"/>
-      <c r="G13" s="40"/>
-      <c r="H13" s="40"/>
-      <c r="I13" s="41"/>
-    </row>
-    <row r="14" spans="2:9" s="1" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="42"/>
-      <c r="C14" s="43"/>
-      <c r="D14" s="43"/>
-      <c r="E14" s="43"/>
-      <c r="F14" s="43"/>
-      <c r="G14" s="43"/>
-      <c r="H14" s="43"/>
-      <c r="I14" s="44"/>
-    </row>
-    <row r="15" spans="2:9" s="1" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="16" spans="2:9" s="1" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="45" t="s">
+      <c r="C13" s="44"/>
+      <c r="D13" s="44"/>
+      <c r="E13" s="44"/>
+      <c r="F13" s="44"/>
+      <c r="G13" s="44"/>
+      <c r="H13" s="44"/>
+      <c r="I13" s="45"/>
+    </row>
+    <row r="14" spans="2:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B14" s="46"/>
+      <c r="C14" s="39"/>
+      <c r="D14" s="39"/>
+      <c r="E14" s="39"/>
+      <c r="F14" s="39"/>
+      <c r="G14" s="39"/>
+      <c r="H14" s="39"/>
+      <c r="I14" s="41"/>
+    </row>
+    <row r="15" spans="2:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="16" spans="2:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B16" s="47" t="s">
         <v>19</v>
       </c>
-      <c r="C16" s="46"/>
-      <c r="D16" s="46"/>
-      <c r="E16" s="46"/>
-      <c r="F16" s="46"/>
-      <c r="G16" s="46"/>
-      <c r="H16" s="46"/>
-      <c r="I16" s="47"/>
-    </row>
-    <row r="17" spans="2:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="48">
+      <c r="C16" s="48"/>
+      <c r="D16" s="48"/>
+      <c r="E16" s="48"/>
+      <c r="F16" s="48"/>
+      <c r="G16" s="48"/>
+      <c r="H16" s="48"/>
+      <c r="I16" s="49"/>
+    </row>
+    <row r="17" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B17" s="14">
         <v>1</v>
       </c>
-      <c r="C17" s="49"/>
-      <c r="D17" s="29"/>
-      <c r="E17" s="50"/>
-      <c r="F17" s="48"/>
-      <c r="G17" s="29"/>
-      <c r="H17" s="27"/>
-      <c r="I17" s="51"/>
-    </row>
-    <row r="18" spans="2:9" s="1" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="52">
+      <c r="C17" s="58"/>
+      <c r="D17" s="36"/>
+      <c r="E17" s="59"/>
+      <c r="F17" s="14"/>
+      <c r="G17" s="36"/>
+      <c r="H17" s="37"/>
+      <c r="I17" s="42"/>
+    </row>
+    <row r="18" spans="2:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B18" s="15">
         <v>2</v>
       </c>
-      <c r="C18" s="43"/>
-      <c r="D18" s="53"/>
-      <c r="E18" s="44"/>
-      <c r="F18" s="52">
+      <c r="C18" s="39"/>
+      <c r="D18" s="40"/>
+      <c r="E18" s="41"/>
+      <c r="F18" s="15">
         <v>3</v>
       </c>
-      <c r="G18" s="43"/>
-      <c r="H18" s="43"/>
-      <c r="I18" s="44"/>
-    </row>
-    <row r="19" spans="2:9" s="1" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="54"/>
-      <c r="F19" s="54"/>
-    </row>
-    <row r="20" spans="2:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="39" t="s">
+      <c r="G18" s="39"/>
+      <c r="H18" s="39"/>
+      <c r="I18" s="41"/>
+    </row>
+    <row r="19" spans="2:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B19" s="16"/>
+      <c r="F19" s="16"/>
+    </row>
+    <row r="20" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B20" s="43" t="s">
         <v>20</v>
       </c>
-      <c r="C20" s="40"/>
-      <c r="D20" s="40"/>
-      <c r="E20" s="40"/>
-      <c r="F20" s="40"/>
-      <c r="G20" s="40"/>
-      <c r="H20" s="40"/>
-      <c r="I20" s="41"/>
-    </row>
-    <row r="21" spans="2:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="5"/>
-      <c r="C21" s="33"/>
-      <c r="D21" s="33"/>
-      <c r="E21" s="33"/>
-      <c r="F21" s="33"/>
-      <c r="G21" s="33"/>
-      <c r="H21" s="33"/>
-      <c r="I21" s="34"/>
-    </row>
-    <row r="22" spans="2:9" s="1" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="18"/>
-      <c r="C22" s="43"/>
-      <c r="D22" s="43"/>
-      <c r="E22" s="43"/>
-      <c r="F22" s="43"/>
-      <c r="G22" s="43"/>
-      <c r="H22" s="43"/>
-      <c r="I22" s="44"/>
-    </row>
-    <row r="23" spans="2:9" s="1" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="24" spans="2:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="39" t="s">
+      <c r="C20" s="44"/>
+      <c r="D20" s="44"/>
+      <c r="E20" s="44"/>
+      <c r="F20" s="44"/>
+      <c r="G20" s="44"/>
+      <c r="H20" s="44"/>
+      <c r="I20" s="45"/>
+    </row>
+    <row r="21" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B21" s="4"/>
+      <c r="C21" s="34"/>
+      <c r="D21" s="34"/>
+      <c r="E21" s="34"/>
+      <c r="F21" s="34"/>
+      <c r="G21" s="34"/>
+      <c r="H21" s="34"/>
+      <c r="I21" s="35"/>
+    </row>
+    <row r="22" spans="2:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B22" s="8"/>
+      <c r="C22" s="39"/>
+      <c r="D22" s="39"/>
+      <c r="E22" s="39"/>
+      <c r="F22" s="39"/>
+      <c r="G22" s="39"/>
+      <c r="H22" s="39"/>
+      <c r="I22" s="41"/>
+    </row>
+    <row r="23" spans="2:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="24" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B24" s="43" t="s">
         <v>21</v>
       </c>
-      <c r="C24" s="40"/>
-      <c r="D24" s="40"/>
-      <c r="E24" s="40"/>
-      <c r="F24" s="40"/>
-      <c r="G24" s="40"/>
-      <c r="H24" s="40"/>
-      <c r="I24" s="41"/>
-    </row>
-    <row r="25" spans="2:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="55" t="s">
+      <c r="C24" s="44"/>
+      <c r="D24" s="44"/>
+      <c r="E24" s="44"/>
+      <c r="F24" s="44"/>
+      <c r="G24" s="44"/>
+      <c r="H24" s="44"/>
+      <c r="I24" s="45"/>
+    </row>
+    <row r="25" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B25" s="51" t="s">
         <v>22</v>
       </c>
-      <c r="C25" s="33"/>
-      <c r="D25" s="33"/>
-      <c r="E25" s="35"/>
-      <c r="F25" s="33" t="s">
+      <c r="C25" s="34"/>
+      <c r="D25" s="34"/>
+      <c r="E25" s="13"/>
+      <c r="F25" s="34" t="s">
         <v>25</v>
       </c>
-      <c r="G25" s="33"/>
-      <c r="H25" s="33"/>
-      <c r="I25" s="34"/>
-    </row>
-    <row r="26" spans="2:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="55" t="s">
+      <c r="G25" s="34"/>
+      <c r="H25" s="34"/>
+      <c r="I25" s="35"/>
+    </row>
+    <row r="26" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B26" s="51" t="s">
         <v>23</v>
       </c>
-      <c r="C26" s="33"/>
-      <c r="D26" s="33"/>
-      <c r="E26" s="35"/>
-      <c r="F26" s="33" t="s">
+      <c r="C26" s="34"/>
+      <c r="D26" s="34"/>
+      <c r="E26" s="13"/>
+      <c r="F26" s="34" t="s">
         <v>26</v>
       </c>
-      <c r="G26" s="33"/>
-      <c r="H26" s="33"/>
-      <c r="I26" s="34"/>
-    </row>
-    <row r="27" spans="2:9" s="1" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B27" s="42" t="s">
+      <c r="G26" s="34"/>
+      <c r="H26" s="34"/>
+      <c r="I26" s="35"/>
+    </row>
+    <row r="27" spans="2:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B27" s="46" t="s">
         <v>24</v>
       </c>
-      <c r="C27" s="43"/>
-      <c r="D27" s="43"/>
-      <c r="E27" s="10"/>
-      <c r="F27" s="43" t="s">
+      <c r="C27" s="39"/>
+      <c r="D27" s="39"/>
+      <c r="E27" s="6"/>
+      <c r="F27" s="39" t="s">
         <v>27</v>
       </c>
-      <c r="G27" s="43"/>
-      <c r="H27" s="43"/>
-      <c r="I27" s="44"/>
-    </row>
-    <row r="28" spans="2:9" s="1" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="29" spans="2:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="39" t="s">
+      <c r="G27" s="39"/>
+      <c r="H27" s="39"/>
+      <c r="I27" s="41"/>
+    </row>
+    <row r="28" spans="2:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="29" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B29" s="43" t="s">
         <v>12</v>
       </c>
-      <c r="C29" s="40"/>
-      <c r="D29" s="40"/>
-      <c r="E29" s="40"/>
-      <c r="F29" s="40"/>
-      <c r="G29" s="40"/>
-      <c r="H29" s="40"/>
-      <c r="I29" s="41"/>
-    </row>
-    <row r="30" spans="2:9" s="1" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B30" s="42"/>
-      <c r="C30" s="43"/>
-      <c r="D30" s="43"/>
-      <c r="E30" s="43"/>
-      <c r="F30" s="43"/>
-      <c r="G30" s="43"/>
-      <c r="H30" s="43"/>
-      <c r="I30" s="44"/>
+      <c r="C29" s="44"/>
+      <c r="D29" s="44"/>
+      <c r="E29" s="44"/>
+      <c r="F29" s="44"/>
+      <c r="G29" s="44"/>
+      <c r="H29" s="44"/>
+      <c r="I29" s="45"/>
+    </row>
+    <row r="30" spans="2:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B30" s="46"/>
+      <c r="C30" s="39"/>
+      <c r="D30" s="39"/>
+      <c r="E30" s="39"/>
+      <c r="F30" s="39"/>
+      <c r="G30" s="39"/>
+      <c r="H30" s="39"/>
+      <c r="I30" s="41"/>
     </row>
   </sheetData>
   <mergeCells count="37">
-    <mergeCell ref="E7:I7"/>
-    <mergeCell ref="E2:H2"/>
-    <mergeCell ref="F5:I5"/>
-    <mergeCell ref="E3:I3"/>
-    <mergeCell ref="E4:I4"/>
-    <mergeCell ref="E6:I6"/>
-    <mergeCell ref="C18:E18"/>
-    <mergeCell ref="G18:I18"/>
-    <mergeCell ref="G17:I17"/>
-    <mergeCell ref="B20:I20"/>
-    <mergeCell ref="B10:I10"/>
-    <mergeCell ref="B11:I11"/>
-    <mergeCell ref="B13:I13"/>
-    <mergeCell ref="B14:I14"/>
-    <mergeCell ref="B16:I16"/>
-    <mergeCell ref="H25:I25"/>
-    <mergeCell ref="H26:I26"/>
-    <mergeCell ref="B24:I24"/>
-    <mergeCell ref="B29:I29"/>
-    <mergeCell ref="B30:I30"/>
-    <mergeCell ref="H27:I27"/>
     <mergeCell ref="B2:D2"/>
     <mergeCell ref="B25:D25"/>
     <mergeCell ref="B26:D26"/>
@@ -2128,9 +2389,159 @@
     <mergeCell ref="C21:I21"/>
     <mergeCell ref="C22:I22"/>
     <mergeCell ref="C17:E17"/>
+    <mergeCell ref="H25:I25"/>
+    <mergeCell ref="H26:I26"/>
+    <mergeCell ref="B24:I24"/>
+    <mergeCell ref="B29:I29"/>
+    <mergeCell ref="B30:I30"/>
+    <mergeCell ref="H27:I27"/>
+    <mergeCell ref="C18:E18"/>
+    <mergeCell ref="G18:I18"/>
+    <mergeCell ref="G17:I17"/>
+    <mergeCell ref="B20:I20"/>
+    <mergeCell ref="B10:I10"/>
+    <mergeCell ref="B11:I11"/>
+    <mergeCell ref="B13:I13"/>
+    <mergeCell ref="B14:I14"/>
+    <mergeCell ref="B16:I16"/>
+    <mergeCell ref="E7:I7"/>
+    <mergeCell ref="E2:H2"/>
+    <mergeCell ref="F5:I5"/>
+    <mergeCell ref="E3:I3"/>
+    <mergeCell ref="E4:I4"/>
+    <mergeCell ref="E6:I6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B3:F13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="11.42578125" style="62"/>
+    <col min="3" max="3" width="3.140625" style="62" customWidth="1"/>
+    <col min="4" max="4" width="34.5703125" style="62" customWidth="1"/>
+    <col min="5" max="5" width="44.42578125" style="62" customWidth="1"/>
+    <col min="6" max="16384" width="11.42578125" style="62"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B3" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+    </row>
+    <row r="4" spans="2:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+    </row>
+    <row r="5" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B5" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="C5" s="10"/>
+      <c r="D5" s="65"/>
+      <c r="E5" s="66"/>
+      <c r="F5" s="1"/>
+    </row>
+    <row r="6" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B6" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="C6" s="12"/>
+      <c r="D6" s="25"/>
+      <c r="E6" s="32"/>
+      <c r="F6" s="1"/>
+    </row>
+    <row r="7" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B7" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="C7" s="12"/>
+      <c r="D7" s="25"/>
+      <c r="E7" s="32"/>
+      <c r="F7" s="1"/>
+    </row>
+    <row r="8" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B8" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="C8" s="12"/>
+      <c r="D8" s="25"/>
+      <c r="E8" s="32"/>
+      <c r="F8" s="1"/>
+    </row>
+    <row r="9" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B9" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" s="12"/>
+      <c r="D9" s="25"/>
+      <c r="E9" s="32"/>
+      <c r="F9" s="1"/>
+    </row>
+    <row r="10" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B10" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="C10" s="12"/>
+      <c r="D10" s="25"/>
+      <c r="E10" s="32"/>
+      <c r="F10" s="1"/>
+    </row>
+    <row r="11" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B11" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="C11" s="12"/>
+      <c r="D11" s="25"/>
+      <c r="E11" s="32"/>
+      <c r="F11" s="1"/>
+    </row>
+    <row r="12" spans="2:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="60" t="s">
+        <v>12</v>
+      </c>
+      <c r="C12" s="61"/>
+      <c r="D12" s="63"/>
+      <c r="E12" s="64"/>
+      <c r="F12" s="1"/>
+    </row>
+    <row r="13" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+    </row>
+  </sheetData>
+  <mergeCells count="8">
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="D11:E11"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" copies="0" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>